<commit_message>
Added lifts to background image and presentation files
</commit_message>
<xml_diff>
--- a/bin/data/runs.xlsx
+++ b/bin/data/runs.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://brightongrammar-my.sharepoint.com/personal/wysssam_brightongrammar_vic_edu_au/Documents/iDesign/SnowWizard/bin/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wysssam\OneDrive - Brighton Grammar School\iDesign\SnowWizard\bin\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="936" yWindow="0" windowWidth="22104" windowHeight="9780"/>
+    <workbookView xWindow="1872" yWindow="0" windowWidth="22104" windowHeight="9780"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="CSS Difficulty Colour" sheetId="1" r:id="rId1"/>
+    <sheet name="Descriptions" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="157">
   <si>
     <t>baldy</t>
   </si>
@@ -465,13 +466,43 @@
   </si>
   <si>
     <t>5dblBlack</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Difficulty</t>
+  </si>
+  <si>
+    <t>Colour</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Easily accessible easier run.</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Bourke St is the main run on the mountain. It is accessed by the Blue Bullet Chair. Many begginners chose this run and lift ques* are usially very large. This is the run that you need to take from the village to get to all the other runs. It is short and always open. Night skiing is held on this run.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baldy is the extention of Bourke St. The Abom Express takes you to the top of Baldy. It is a long wide run. Blady's chair takes you to up so you can access all the other runs on the mountain. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -479,13 +510,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -500,8 +552,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -782,41 +836,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D1:J71"/>
+  <dimension ref="A1:K72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J71"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="8" max="8" width="47.77734375" customWidth="1"/>
     <col min="10" max="10" width="53.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="K1" s="2"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
         <v>56</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" t="s">
         <v>57</v>
-      </c>
-      <c r="F1">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>142</v>
-      </c>
-      <c r="J1" t="str">
-        <f>"g#"&amp;D1&amp;" path , g#"&amp;D1&amp;" line , g#"&amp;D1&amp;" polyline ,"</f>
-        <v>g#gliders path , g#gliders line , g#gliders polyline ,</v>
-      </c>
-    </row>
-    <row r="2" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" t="s">
-        <v>59</v>
       </c>
       <c r="F2">
         <v>5</v>
@@ -825,88 +887,94 @@
         <v>142</v>
       </c>
       <c r="J2" t="str">
-        <f t="shared" ref="J2:J65" si="0">"g#"&amp;D2&amp;" path , g#"&amp;D2&amp;" line , g#"&amp;D2&amp;" polyline ,"</f>
+        <f>"g#"&amp;D2&amp;" path , g#"&amp;D2&amp;" line , g#"&amp;D2&amp;" polyline ,"</f>
+        <v>g#gliders path , g#gliders line , g#gliders polyline ,</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>142</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J66" si="0">"g#"&amp;D3&amp;" path , g#"&amp;D3&amp;" line , g#"&amp;D3&amp;" polyline ,"</f>
         <v>g#happyfeet path , g#happyfeet line , g#happyfeet polyline ,</v>
       </c>
     </row>
-    <row r="3" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D3" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>13</v>
       </c>
-      <c r="F3">
+      <c r="F4">
         <v>20</v>
-      </c>
-      <c r="G3" t="s">
-        <v>143</v>
-      </c>
-      <c r="J3" t="str">
-        <f t="shared" si="0"/>
-        <v>g#bourkest path , g#bourkest line , g#bourkest polyline ,</v>
-      </c>
-    </row>
-    <row r="4" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>25</v>
       </c>
       <c r="G4" t="s">
         <v>143</v>
       </c>
+      <c r="H4" t="s">
+        <v>155</v>
+      </c>
       <c r="J4" t="str">
         <f t="shared" si="0"/>
-        <v>g#baldy path , g#baldy line , g#baldy polyline ,</v>
-      </c>
-    </row>
-    <row r="5" spans="4:10" x14ac:dyDescent="0.3">
+        <v>g#bourkest path , g#bourkest line , g#bourkest polyline ,</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G5" t="s">
         <v>143</v>
       </c>
+      <c r="H5" t="s">
+        <v>156</v>
+      </c>
       <c r="J5" t="str">
         <f t="shared" si="0"/>
+        <v>g#baldy path , g#baldy line , g#baldy polyline ,</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s">
+        <v>143</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="0"/>
         <v>g#burnthutspur path , g#burnthutspur line , g#burnthutspur polyline ,</v>
       </c>
     </row>
-    <row r="6" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D6" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
         <v>46</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>47</v>
-      </c>
-      <c r="F6">
-        <v>35</v>
-      </c>
-      <c r="G6" t="s">
-        <v>144</v>
-      </c>
-      <c r="J6" t="str">
-        <f t="shared" si="0"/>
-        <v>g#familyrun path , g#familyrun line , g#familyrun polyline ,</v>
-      </c>
-    </row>
-    <row r="7" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D7" t="s">
-        <v>92</v>
-      </c>
-      <c r="E7" t="s">
-        <v>93</v>
       </c>
       <c r="F7">
         <v>35</v>
@@ -916,33 +984,33 @@
       </c>
       <c r="J7" t="str">
         <f t="shared" si="0"/>
+        <v>g#familyrun path , g#familyrun line , g#familyrun polyline ,</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F8">
+        <v>35</v>
+      </c>
+      <c r="G8" t="s">
+        <v>144</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="0"/>
         <v>g#skyline path , g#skyline line , g#skyline polyline ,</v>
       </c>
     </row>
-    <row r="8" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D8" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
         <v>20</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>21</v>
-      </c>
-      <c r="F8">
-        <v>40</v>
-      </c>
-      <c r="G8" t="s">
-        <v>144</v>
-      </c>
-      <c r="J8" t="str">
-        <f t="shared" si="0"/>
-        <v>g#canyontrail path , g#canyontrail line , g#canyontrail polyline ,</v>
-      </c>
-    </row>
-    <row r="9" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" t="s">
-        <v>53</v>
       </c>
       <c r="F9">
         <v>40</v>
@@ -952,15 +1020,15 @@
       </c>
       <c r="J9" t="str">
         <f t="shared" si="0"/>
-        <v>g#foxaccess path , g#foxaccess line , g#foxaccess polyline ,</v>
-      </c>
-    </row>
-    <row r="10" spans="4:10" x14ac:dyDescent="0.3">
+        <v>g#canyontrail path , g#canyontrail line , g#canyontrail polyline ,</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="E10" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="F10">
         <v>40</v>
@@ -970,15 +1038,15 @@
       </c>
       <c r="J10" t="str">
         <f t="shared" si="0"/>
-        <v>g#hometrail path , g#hometrail line , g#hometrail polyline ,</v>
-      </c>
-    </row>
-    <row r="11" spans="4:10" x14ac:dyDescent="0.3">
+        <v>g#foxaccess path , g#foxaccess line , g#foxaccess polyline ,</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
-        <v>100</v>
+        <v>62</v>
       </c>
       <c r="E11" t="s">
-        <v>101</v>
+        <v>63</v>
       </c>
       <c r="F11">
         <v>40</v>
@@ -988,15 +1056,15 @@
       </c>
       <c r="J11" t="str">
         <f t="shared" si="0"/>
-        <v>g#summitaccess path , g#summitaccess line , g#summitaccess polyline ,</v>
-      </c>
-    </row>
-    <row r="12" spans="4:10" x14ac:dyDescent="0.3">
+        <v>g#hometrail path , g#hometrail line , g#hometrail polyline ,</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="E12" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="F12">
         <v>40</v>
@@ -1006,33 +1074,33 @@
       </c>
       <c r="J12" t="str">
         <f t="shared" si="0"/>
+        <v>g#summitaccess path , g#summitaccess line , g#summitaccess polyline ,</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E13" t="s">
+        <v>125</v>
+      </c>
+      <c r="F13">
+        <v>40</v>
+      </c>
+      <c r="G13" t="s">
+        <v>144</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="0"/>
         <v>g#whiskeycreektrail path , g#whiskeycreektrail line , g#whiskeycreektrail polyline ,</v>
       </c>
     </row>
-    <row r="13" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D13" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
         <v>90</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>91</v>
-      </c>
-      <c r="F13">
-        <v>45</v>
-      </c>
-      <c r="G13" t="s">
-        <v>144</v>
-      </c>
-      <c r="J13" t="str">
-        <f t="shared" si="0"/>
-        <v>g#shakeyknees path , g#shakeyknees line , g#shakeyknees polyline ,</v>
-      </c>
-    </row>
-    <row r="14" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D14" t="s">
-        <v>98</v>
-      </c>
-      <c r="E14" t="s">
-        <v>99</v>
       </c>
       <c r="F14">
         <v>45</v>
@@ -1042,33 +1110,33 @@
       </c>
       <c r="J14" t="str">
         <f t="shared" si="0"/>
+        <v>g#shakeyknees path , g#shakeyknees line , g#shakeyknees polyline ,</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>98</v>
+      </c>
+      <c r="E15" t="s">
+        <v>99</v>
+      </c>
+      <c r="F15">
+        <v>45</v>
+      </c>
+      <c r="G15" t="s">
+        <v>144</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="0"/>
         <v>g#summit path , g#summit line , g#summit polyline ,</v>
       </c>
     </row>
-    <row r="15" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D15" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
         <v>2</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E16" t="s">
         <v>3</v>
-      </c>
-      <c r="F15">
-        <v>50</v>
-      </c>
-      <c r="G15" t="s">
-        <v>144</v>
-      </c>
-      <c r="J15" t="str">
-        <f t="shared" si="0"/>
-        <v>g#blizzardracecourse path , g#blizzardracecourse line , g#blizzardracecourse polyline ,</v>
-      </c>
-    </row>
-    <row r="16" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" t="s">
-        <v>9</v>
       </c>
       <c r="F16">
         <v>50</v>
@@ -1078,15 +1146,15 @@
       </c>
       <c r="J16" t="str">
         <f t="shared" si="0"/>
-        <v>g#boomerang path , g#boomerang line , g#boomerang polyline ,</v>
+        <v>g#blizzardracecourse path , g#blizzardracecourse line , g#blizzardracecourse polyline ,</v>
       </c>
     </row>
     <row r="17" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="E17" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="F17">
         <v>50</v>
@@ -1096,15 +1164,15 @@
       </c>
       <c r="J17" t="str">
         <f t="shared" si="0"/>
-        <v>g#colt path , g#colt line , g#colt polyline ,</v>
+        <v>g#boomerang path , g#boomerang line , g#boomerang polyline ,</v>
       </c>
     </row>
     <row r="18" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
-        <v>68</v>
+        <v>30</v>
       </c>
       <c r="E18" t="s">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="F18">
         <v>50</v>
@@ -1114,15 +1182,15 @@
       </c>
       <c r="J18" t="str">
         <f t="shared" si="0"/>
-        <v>g#littlebullerspur path , g#littlebullerspur line , g#littlebullerspur polyline ,</v>
+        <v>g#colt path , g#colt line , g#colt polyline ,</v>
       </c>
     </row>
     <row r="19" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
-        <v>110</v>
+        <v>68</v>
       </c>
       <c r="E19" t="s">
-        <v>111</v>
+        <v>69</v>
       </c>
       <c r="F19">
         <v>50</v>
@@ -1132,15 +1200,15 @@
       </c>
       <c r="J19" t="str">
         <f t="shared" si="0"/>
-        <v>g#tirol path , g#tirol line , g#tirol polyline ,</v>
+        <v>g#littlebullerspur path , g#littlebullerspur line , g#littlebullerspur polyline ,</v>
       </c>
     </row>
     <row r="20" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="E20" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="F20">
         <v>50</v>
@@ -1150,15 +1218,15 @@
       </c>
       <c r="J20" t="str">
         <f t="shared" si="0"/>
-        <v>g#wenzelsweave path , g#wenzelsweave line , g#wenzelsweave polyline ,</v>
+        <v>g#tirol path , g#tirol line , g#tirol polyline ,</v>
       </c>
     </row>
     <row r="21" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="E21" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F21">
         <v>50</v>
@@ -1168,33 +1236,33 @@
       </c>
       <c r="J21" t="str">
         <f t="shared" si="0"/>
-        <v>g#wombat path , g#wombat line , g#wombat polyline ,</v>
+        <v>g#wenzelsweave path , g#wenzelsweave line , g#wenzelsweave polyline ,</v>
       </c>
     </row>
     <row r="22" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
-        <v>6</v>
+        <v>130</v>
       </c>
       <c r="E22" t="s">
-        <v>7</v>
+        <v>131</v>
       </c>
       <c r="F22">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="G22" t="s">
         <v>144</v>
       </c>
       <c r="J22" t="str">
         <f t="shared" si="0"/>
-        <v>g#boggycreek path , g#boggycreek line , g#boggycreek polyline ,</v>
+        <v>g#wombat path , g#wombat line , g#wombat polyline ,</v>
       </c>
     </row>
     <row r="23" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E23" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F23">
         <v>55</v>
@@ -1204,15 +1272,15 @@
       </c>
       <c r="J23" t="str">
         <f t="shared" si="0"/>
-        <v>g#brumby path , g#brumby line , g#brumby polyline ,</v>
+        <v>g#boggycreek path , g#boggycreek line , g#boggycreek polyline ,</v>
       </c>
     </row>
     <row r="24" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E24" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="F24">
         <v>55</v>
@@ -1222,15 +1290,15 @@
       </c>
       <c r="J24" t="str">
         <f t="shared" si="0"/>
-        <v>g#chute path , g#chute line , g#chute polyline ,</v>
+        <v>g#brumby path , g#brumby line , g#brumby polyline ,</v>
       </c>
     </row>
     <row r="25" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E25" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F25">
         <v>55</v>
@@ -1240,15 +1308,15 @@
       </c>
       <c r="J25" t="str">
         <f t="shared" si="0"/>
-        <v>g#crosscut path , g#crosscut line , g#crosscut polyline ,</v>
+        <v>g#chute path , g#chute line , g#chute polyline ,</v>
       </c>
     </row>
     <row r="26" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D26" t="s">
-        <v>96</v>
+        <v>34</v>
       </c>
       <c r="E26" t="s">
-        <v>97</v>
+        <v>35</v>
       </c>
       <c r="F26">
         <v>55</v>
@@ -1258,15 +1326,15 @@
       </c>
       <c r="J26" t="str">
         <f t="shared" si="0"/>
-        <v>g#standard path , g#standard line , g#standard polyline ,</v>
+        <v>g#crosscut path , g#crosscut line , g#crosscut polyline ,</v>
       </c>
     </row>
     <row r="27" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D27" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="E27" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="F27">
         <v>55</v>
@@ -1276,15 +1344,15 @@
       </c>
       <c r="J27" t="str">
         <f t="shared" si="0"/>
-        <v>g#vista path , g#vista line , g#vista polyline ,</v>
+        <v>g#standard path , g#standard line , g#standard polyline ,</v>
       </c>
     </row>
     <row r="28" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E28" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F28">
         <v>55</v>
@@ -1294,15 +1362,15 @@
       </c>
       <c r="J28" t="str">
         <f t="shared" si="0"/>
-        <v>g#waler path , g#waler line , g#waler polyline ,</v>
+        <v>g#vista path , g#vista line , g#vista polyline ,</v>
       </c>
     </row>
     <row r="29" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D29" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="E29" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="F29">
         <v>55</v>
@@ -1312,51 +1380,51 @@
       </c>
       <c r="J29" t="str">
         <f t="shared" si="0"/>
-        <v>g#windlessmarissa path , g#windlessmarissa line , g#windlessmarissa polyline ,</v>
+        <v>g#waler path , g#waler line , g#waler polyline ,</v>
       </c>
     </row>
     <row r="30" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
-        <v>66</v>
+        <v>126</v>
       </c>
       <c r="E30" t="s">
-        <v>67</v>
+        <v>127</v>
       </c>
       <c r="F30">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G30" t="s">
         <v>144</v>
       </c>
       <c r="J30" t="str">
         <f t="shared" si="0"/>
-        <v>g#laycockslane path , g#laycockslane line , g#laycockslane polyline ,</v>
+        <v>g#windlessmarissa path , g#windlessmarissa line , g#windlessmarissa polyline ,</v>
       </c>
     </row>
     <row r="31" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D31" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="E31" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="F31">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G31" t="s">
         <v>144</v>
       </c>
       <c r="J31" t="str">
         <f t="shared" si="0"/>
-        <v>g#cattlemanstrail path , g#cattlemanstrail line , g#cattlemanstrail polyline ,</v>
+        <v>g#laycockslane path , g#laycockslane line , g#laycockslane polyline ,</v>
       </c>
     </row>
     <row r="32" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D32" t="s">
-        <v>104</v>
+        <v>22</v>
       </c>
       <c r="E32" t="s">
-        <v>105</v>
+        <v>23</v>
       </c>
       <c r="F32">
         <v>60</v>
@@ -1366,51 +1434,51 @@
       </c>
       <c r="J32" t="str">
         <f t="shared" si="0"/>
-        <v>g#summitslide path , g#summitslide line , g#summitslide polyline ,</v>
+        <v>g#cattlemanstrail path , g#cattlemanstrail line , g#cattlemanstrail polyline ,</v>
       </c>
     </row>
     <row r="33" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D33" t="s">
-        <v>26</v>
+        <v>104</v>
       </c>
       <c r="E33" t="s">
-        <v>27</v>
+        <v>105</v>
       </c>
       <c r="F33">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="G33" t="s">
         <v>144</v>
       </c>
       <c r="J33" t="str">
         <f t="shared" si="0"/>
-        <v>g#chamois path , g#chamois line , g#chamois polyline ,</v>
+        <v>g#summitslide path , g#summitslide line , g#summitslide polyline ,</v>
       </c>
     </row>
     <row r="34" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D34" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E34" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F34">
         <v>70</v>
       </c>
       <c r="G34" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J34" t="str">
         <f t="shared" si="0"/>
-        <v>g#cowcamp path , g#cowcamp line , g#cowcamp polyline ,</v>
+        <v>g#chamois path , g#chamois line , g#chamois polyline ,</v>
       </c>
     </row>
     <row r="35" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D35" t="s">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="E35" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="F35">
         <v>70</v>
@@ -1420,15 +1488,15 @@
       </c>
       <c r="J35" t="str">
         <f t="shared" si="0"/>
-        <v>g#howqua path , g#howqua line , g#howqua polyline ,</v>
+        <v>g#cowcamp path , g#cowcamp line , g#cowcamp polyline ,</v>
       </c>
     </row>
     <row r="36" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D36" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="E36" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="F36">
         <v>70</v>
@@ -1438,15 +1506,15 @@
       </c>
       <c r="J36" t="str">
         <f t="shared" si="0"/>
-        <v>g#stchristopher path , g#stchristopher line , g#stchristopher polyline ,</v>
+        <v>g#howqua path , g#howqua line , g#howqua polyline ,</v>
       </c>
     </row>
     <row r="37" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D37" t="s">
-        <v>114</v>
+        <v>86</v>
       </c>
       <c r="E37" t="s">
-        <v>115</v>
+        <v>87</v>
       </c>
       <c r="F37">
         <v>70</v>
@@ -1456,15 +1524,15 @@
       </c>
       <c r="J37" t="str">
         <f t="shared" si="0"/>
-        <v>g#village path , g#village line , g#village polyline ,</v>
+        <v>g#stchristopher path , g#stchristopher line , g#stchristopher polyline ,</v>
       </c>
     </row>
     <row r="38" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D38" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="E38" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F38">
         <v>70</v>
@@ -1474,15 +1542,15 @@
       </c>
       <c r="J38" t="str">
         <f t="shared" si="0"/>
-        <v>g#wattlewiggle path , g#wattlewiggle line , g#wattlewiggle polyline ,</v>
+        <v>g#village path , g#village line , g#village polyline ,</v>
       </c>
     </row>
     <row r="39" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D39" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="E39" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="F39">
         <v>70</v>
@@ -1492,15 +1560,15 @@
       </c>
       <c r="J39" t="str">
         <f t="shared" si="0"/>
-        <v>g#wombatbottomroad path , g#wombatbottomroad line , g#wombatbottomroad polyline ,</v>
+        <v>g#wattlewiggle path , g#wattlewiggle line , g#wattlewiggle polyline ,</v>
       </c>
     </row>
     <row r="40" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D40" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E40" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F40">
         <v>70</v>
@@ -1510,33 +1578,33 @@
       </c>
       <c r="J40" t="str">
         <f t="shared" si="0"/>
-        <v>g#wombatmidroad path , g#wombatmidroad line , g#wombatmidroad polyline ,</v>
+        <v>g#wombatbottomroad path , g#wombatbottomroad line , g#wombatbottomroad polyline ,</v>
       </c>
     </row>
     <row r="41" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D41" t="s">
-        <v>10</v>
+        <v>134</v>
       </c>
       <c r="E41" t="s">
-        <v>11</v>
+        <v>135</v>
       </c>
       <c r="F41">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="G41" t="s">
         <v>145</v>
       </c>
       <c r="J41" t="str">
         <f t="shared" si="0"/>
-        <v>g#boulders path , g#boulders line , g#boulders polyline ,</v>
+        <v>g#wombatmidroad path , g#wombatmidroad line , g#wombatmidroad polyline ,</v>
       </c>
     </row>
     <row r="42" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D42" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="E42" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F42">
         <v>75</v>
@@ -1546,15 +1614,15 @@
       </c>
       <c r="J42" t="str">
         <f t="shared" si="0"/>
-        <v>g#chaletcreek path , g#chaletcreek line , g#chaletcreek polyline ,</v>
+        <v>g#boulders path , g#boulders line , g#boulders polyline ,</v>
       </c>
     </row>
     <row r="43" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D43" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="E43" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="F43">
         <v>75</v>
@@ -1564,15 +1632,15 @@
       </c>
       <c r="J43" t="str">
         <f t="shared" si="0"/>
-        <v>g#damrun path , g#damrun line , g#damrun polyline ,</v>
+        <v>g#chaletcreek path , g#chaletcreek line , g#chaletcreek polyline ,</v>
       </c>
     </row>
     <row r="44" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D44" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E44" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F44">
         <v>75</v>
@@ -1582,15 +1650,15 @@
       </c>
       <c r="J44" t="str">
         <f t="shared" si="0"/>
-        <v>g#elephantrun path , g#elephantrun line , g#elephantrun polyline ,</v>
+        <v>g#damrun path , g#damrun line , g#damrun polyline ,</v>
       </c>
     </row>
     <row r="45" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D45" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="E45" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="F45">
         <v>75</v>
@@ -1600,15 +1668,15 @@
       </c>
       <c r="J45" t="str">
         <f t="shared" si="0"/>
-        <v>g#hoggsback path , g#hoggsback line , g#hoggsback polyline ,</v>
+        <v>g#elephantrun path , g#elephantrun line , g#elephantrun polyline ,</v>
       </c>
     </row>
     <row r="46" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D46" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="E46" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="F46">
         <v>75</v>
@@ -1618,15 +1686,15 @@
       </c>
       <c r="J46" t="str">
         <f t="shared" si="0"/>
-        <v>g#mensdownhill path , g#mensdownhill line , g#mensdownhill polyline ,</v>
+        <v>g#hoggsback path , g#hoggsback line , g#hoggsback polyline ,</v>
       </c>
     </row>
     <row r="47" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D47" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="E47" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="F47">
         <v>75</v>
@@ -1636,15 +1704,15 @@
       </c>
       <c r="J47" t="str">
         <f t="shared" si="0"/>
-        <v>g#roughcut path , g#roughcut line , g#roughcut polyline ,</v>
+        <v>g#mensdownhill path , g#mensdownhill line , g#mensdownhill polyline ,</v>
       </c>
     </row>
     <row r="48" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D48" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E48" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F48">
         <v>75</v>
@@ -1654,15 +1722,15 @@
       </c>
       <c r="J48" t="str">
         <f t="shared" si="0"/>
-        <v>g#scvhutrun path , g#scvhutrun line , g#scvhutrun polyline ,</v>
+        <v>g#roughcut path , g#roughcut line , g#roughcut polyline ,</v>
       </c>
     </row>
     <row r="49" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D49" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="E49" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="F49">
         <v>75</v>
@@ -1672,15 +1740,15 @@
       </c>
       <c r="J49" t="str">
         <f t="shared" si="0"/>
-        <v>g#summitblack path , g#summitblack line , g#summitblack polyline ,</v>
+        <v>g#scvhutrun path , g#scvhutrun line , g#scvhutrun polyline ,</v>
       </c>
     </row>
     <row r="50" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D50" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E50" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F50">
         <v>75</v>
@@ -1690,15 +1758,15 @@
       </c>
       <c r="J50" t="str">
         <f t="shared" si="0"/>
-        <v>g#sunvalley path , g#sunvalley line , g#sunvalley polyline ,</v>
+        <v>g#summitblack path , g#summitblack line , g#summitblack polyline ,</v>
       </c>
     </row>
     <row r="51" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D51" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="E51" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="F51">
         <v>75</v>
@@ -1708,15 +1776,15 @@
       </c>
       <c r="J51" t="str">
         <f t="shared" si="0"/>
-        <v>g#womensdownhill path , g#womensdownhill line , g#womensdownhill polyline ,</v>
+        <v>g#sunvalley path , g#sunvalley line , g#sunvalley polyline ,</v>
       </c>
     </row>
     <row r="52" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D52" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="E52" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="F52">
         <v>75</v>
@@ -1726,33 +1794,33 @@
       </c>
       <c r="J52" t="str">
         <f t="shared" si="0"/>
-        <v>g#yurredla path , g#yurredla line , g#yurredla polyline ,</v>
+        <v>g#womensdownhill path , g#womensdownhill line , g#womensdownhill polyline ,</v>
       </c>
     </row>
     <row r="53" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D53" t="s">
-        <v>74</v>
+        <v>138</v>
       </c>
       <c r="E53" t="s">
+        <v>139</v>
+      </c>
+      <c r="F53">
         <v>75</v>
       </c>
-      <c r="F53">
-        <v>78</v>
-      </c>
       <c r="G53" t="s">
         <v>145</v>
       </c>
       <c r="J53" t="str">
         <f t="shared" si="0"/>
-        <v>g#plughole path , g#plughole line , g#plughole polyline ,</v>
+        <v>g#yurredla path , g#yurredla line , g#yurredla polyline ,</v>
       </c>
     </row>
     <row r="54" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D54" t="s">
-        <v>136</v>
+        <v>74</v>
       </c>
       <c r="E54" t="s">
-        <v>137</v>
+        <v>75</v>
       </c>
       <c r="F54">
         <v>78</v>
@@ -1762,33 +1830,33 @@
       </c>
       <c r="J54" t="str">
         <f t="shared" si="0"/>
-        <v>g#woodrun path , g#woodrun line , g#woodrun polyline ,</v>
+        <v>g#plughole path , g#plughole line , g#plughole polyline ,</v>
       </c>
     </row>
     <row r="55" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D55" t="s">
-        <v>18</v>
+        <v>136</v>
       </c>
       <c r="E55" t="s">
-        <v>19</v>
+        <v>137</v>
       </c>
       <c r="F55">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G55" t="s">
         <v>145</v>
       </c>
       <c r="J55" t="str">
         <f t="shared" si="0"/>
-        <v>g#bullrun path , g#bullrun line , g#bullrun polyline ,</v>
+        <v>g#woodrun path , g#woodrun line , g#woodrun polyline ,</v>
       </c>
     </row>
     <row r="56" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D56" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="E56" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="F56">
         <v>80</v>
@@ -1798,15 +1866,15 @@
       </c>
       <c r="J56" t="str">
         <f t="shared" si="0"/>
-        <v>g#fallline path , g#fallline line , g#fallline polyline ,</v>
+        <v>g#bullrun path , g#bullrun line , g#bullrun polyline ,</v>
       </c>
     </row>
     <row r="57" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D57" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E57" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F57">
         <v>80</v>
@@ -1816,15 +1884,15 @@
       </c>
       <c r="J57" t="str">
         <f t="shared" si="0"/>
-        <v>g#funnel path , g#funnel line , g#funnel polyline ,</v>
+        <v>g#fallline path , g#fallline line , g#fallline polyline ,</v>
       </c>
     </row>
     <row r="58" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D58" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="E58" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="F58">
         <v>80</v>
@@ -1834,15 +1902,15 @@
       </c>
       <c r="J58" t="str">
         <f t="shared" si="0"/>
-        <v>g#rushrun path , g#rushrun line , g#rushrun polyline ,</v>
+        <v>g#funnel path , g#funnel line , g#funnel polyline ,</v>
       </c>
     </row>
     <row r="59" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D59" t="s">
-        <v>140</v>
+        <v>84</v>
       </c>
       <c r="E59" t="s">
-        <v>141</v>
+        <v>85</v>
       </c>
       <c r="F59">
         <v>80</v>
@@ -1852,33 +1920,33 @@
       </c>
       <c r="J59" t="str">
         <f t="shared" si="0"/>
-        <v>g#zwierszigzag path , g#zwierszigzag line , g#zwierszigzag polyline ,</v>
+        <v>g#rushrun path , g#rushrun line , g#rushrun polyline ,</v>
       </c>
     </row>
     <row r="60" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D60" t="s">
-        <v>4</v>
+        <v>140</v>
       </c>
       <c r="E60" t="s">
-        <v>5</v>
+        <v>141</v>
       </c>
       <c r="F60">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G60" t="s">
         <v>145</v>
       </c>
       <c r="J60" t="str">
         <f t="shared" si="0"/>
-        <v>g#bloodyhell path , g#bloodyhell line , g#bloodyhell polyline ,</v>
+        <v>g#zwierszigzag path , g#zwierszigzag line , g#zwierszigzag polyline ,</v>
       </c>
     </row>
     <row r="61" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D61" t="s">
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="E61" t="s">
-        <v>49</v>
+        <v>5</v>
       </c>
       <c r="F61">
         <v>85</v>
@@ -1888,15 +1956,15 @@
       </c>
       <c r="J61" t="str">
         <f t="shared" si="0"/>
-        <v>g#fastone path , g#fastone line , g#fastone polyline ,</v>
+        <v>g#bloodyhell path , g#bloodyhell line , g#bloodyhell polyline ,</v>
       </c>
     </row>
     <row r="62" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D62" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E62" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F62">
         <v>85</v>
@@ -1906,15 +1974,15 @@
       </c>
       <c r="J62" t="str">
         <f t="shared" si="0"/>
-        <v>g#federation path , g#federation line , g#federation polyline ,</v>
+        <v>g#fastone path , g#fastone line , g#fastone polyline ,</v>
       </c>
     </row>
     <row r="63" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D63" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="E63" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="F63">
         <v>85</v>
@@ -1924,15 +1992,15 @@
       </c>
       <c r="J63" t="str">
         <f t="shared" si="0"/>
-        <v>g#outeredge path , g#outeredge line , g#outeredge polyline ,</v>
+        <v>g#federation path , g#federation line , g#federation polyline ,</v>
       </c>
     </row>
     <row r="64" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D64" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E64" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F64">
         <v>85</v>
@@ -1942,15 +2010,15 @@
       </c>
       <c r="J64" t="str">
         <f t="shared" si="0"/>
-        <v>g#ridgerun path , g#ridgerun line , g#ridgerun polyline ,</v>
+        <v>g#outeredge path , g#outeredge line , g#outeredge polyline ,</v>
       </c>
     </row>
     <row r="65" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D65" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="E65" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="F65">
         <v>85</v>
@@ -1960,15 +2028,15 @@
       </c>
       <c r="J65" t="str">
         <f t="shared" si="0"/>
-        <v>g#slalomgully path , g#slalomgully line , g#slalomgully polyline ,</v>
+        <v>g#ridgerun path , g#ridgerun line , g#ridgerun polyline ,</v>
       </c>
     </row>
     <row r="66" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D66" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="E66" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="F66">
         <v>85</v>
@@ -1977,96 +2045,114 @@
         <v>145</v>
       </c>
       <c r="J66" t="str">
-        <f t="shared" ref="J66:J71" si="1">"g#"&amp;D66&amp;" path , g#"&amp;D66&amp;" line , g#"&amp;D66&amp;" polyline ,"</f>
-        <v>g#thulkes path , g#thulkes line , g#thulkes polyline ,</v>
+        <f t="shared" si="0"/>
+        <v>g#slalomgully path , g#slalomgully line , g#slalomgully polyline ,</v>
       </c>
     </row>
     <row r="67" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D67" t="s">
+        <v>112</v>
+      </c>
+      <c r="E67" t="s">
+        <v>113</v>
+      </c>
+      <c r="F67">
+        <v>85</v>
+      </c>
+      <c r="G67" t="s">
+        <v>145</v>
+      </c>
+      <c r="J67" t="str">
+        <f t="shared" ref="J67:J72" si="1">"g#"&amp;D67&amp;" path , g#"&amp;D67&amp;" line , g#"&amp;D67&amp;" polyline ,"</f>
+        <v>g#thulkes path , g#thulkes line , g#thulkes polyline ,</v>
+      </c>
+    </row>
+    <row r="68" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D68" t="s">
         <v>36</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E68" t="s">
         <v>37</v>
       </c>
-      <c r="F67">
+      <c r="F68">
         <v>90</v>
       </c>
-      <c r="G67" t="s">
-        <v>145</v>
-      </c>
-      <c r="J67" t="str">
+      <c r="G68" t="s">
+        <v>145</v>
+      </c>
+      <c r="J68" t="str">
         <f t="shared" si="1"/>
         <v>g#cut73 path , g#cut73 line , g#cut73 polyline ,</v>
       </c>
     </row>
-    <row r="68" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D68" t="s">
+    <row r="69" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D69" t="s">
         <v>76</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E69" t="s">
         <v>77</v>
       </c>
-      <c r="F68">
+      <c r="F69">
         <v>90</v>
       </c>
-      <c r="G68" t="s">
-        <v>145</v>
-      </c>
-      <c r="J68" t="str">
+      <c r="G69" t="s">
+        <v>145</v>
+      </c>
+      <c r="J69" t="str">
         <f t="shared" si="1"/>
         <v>g#powderkeg path , g#powderkeg line , g#powderkeg polyline ,</v>
       </c>
     </row>
-    <row r="69" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D69" t="s">
+    <row r="70" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D70" t="s">
         <v>80</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E70" t="s">
         <v>81</v>
       </c>
-      <c r="F69">
+      <c r="F70">
         <v>90</v>
       </c>
-      <c r="G69" t="s">
-        <v>145</v>
-      </c>
-      <c r="J69" t="str">
+      <c r="G70" t="s">
+        <v>145</v>
+      </c>
+      <c r="J70" t="str">
         <f t="shared" si="1"/>
         <v>g#robins path , g#robins line , g#robins polyline ,</v>
       </c>
     </row>
-    <row r="70" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D70" t="s">
+    <row r="71" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D71" t="s">
         <v>44</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E71" t="s">
         <v>45</v>
       </c>
-      <c r="F70">
+      <c r="F71">
         <v>95</v>
       </c>
-      <c r="G70" t="s">
+      <c r="G71" t="s">
         <v>146</v>
       </c>
-      <c r="J70" t="str">
+      <c r="J71" t="str">
         <f t="shared" si="1"/>
         <v>g#fannysfinish path , g#fannysfinish line , g#fannysfinish polyline ,</v>
       </c>
     </row>
-    <row r="71" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D71" t="s">
+    <row r="72" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D72" t="s">
         <v>108</v>
       </c>
-      <c r="E71" t="s">
+      <c r="E72" t="s">
         <v>109</v>
       </c>
-      <c r="F71">
+      <c r="F72">
         <v>95</v>
       </c>
-      <c r="G71" t="s">
+      <c r="G72" t="s">
         <v>146</v>
       </c>
-      <c r="J71" t="str">
+      <c r="J72" t="str">
         <f t="shared" si="1"/>
         <v>g#thechutes path , g#thechutes line , g#thechutes polyline ,</v>
       </c>
@@ -2077,4 +2163,1041 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F72"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="109.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>25</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1">
+        <v>50</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1">
+        <v>85</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1">
+        <v>55</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1">
+        <v>50</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1">
+        <v>75</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1">
+        <v>20</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="1">
+        <v>55</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="1">
+        <v>80</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="1">
+        <v>30</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="1">
+        <v>40</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="1">
+        <v>60</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="1">
+        <v>75</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="1">
+        <v>70</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="1">
+        <v>55</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="1">
+        <v>50</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="1">
+        <v>70</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="1">
+        <v>55</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="1">
+        <v>90</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="1">
+        <v>75</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="1">
+        <v>75</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="1">
+        <v>80</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="1">
+        <v>35</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="1">
+        <v>95</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="1">
+        <v>85</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="1">
+        <v>85</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" s="1">
+        <v>40</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" s="1">
+        <v>80</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" t="s">
+        <v>57</v>
+      </c>
+      <c r="D30" s="1">
+        <v>5</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" s="1">
+        <v>5</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" s="1">
+        <v>75</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" t="s">
+        <v>63</v>
+      </c>
+      <c r="D33" s="1">
+        <v>40</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" s="1">
+        <v>70</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" t="s">
+        <v>67</v>
+      </c>
+      <c r="D35" s="1">
+        <v>58</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" t="s">
+        <v>69</v>
+      </c>
+      <c r="D36" s="1">
+        <v>50</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" t="s">
+        <v>71</v>
+      </c>
+      <c r="D37" s="1">
+        <v>75</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>72</v>
+      </c>
+      <c r="C38" t="s">
+        <v>73</v>
+      </c>
+      <c r="D38" s="1">
+        <v>85</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" t="s">
+        <v>75</v>
+      </c>
+      <c r="D39" s="1">
+        <v>78</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40" t="s">
+        <v>77</v>
+      </c>
+      <c r="D40" s="1">
+        <v>90</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41" t="s">
+        <v>79</v>
+      </c>
+      <c r="D41" s="1">
+        <v>85</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>80</v>
+      </c>
+      <c r="C42" t="s">
+        <v>81</v>
+      </c>
+      <c r="D42" s="1">
+        <v>90</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>82</v>
+      </c>
+      <c r="C43" t="s">
+        <v>83</v>
+      </c>
+      <c r="D43" s="1">
+        <v>75</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>84</v>
+      </c>
+      <c r="C44" t="s">
+        <v>85</v>
+      </c>
+      <c r="D44" s="1">
+        <v>80</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>88</v>
+      </c>
+      <c r="C45" t="s">
+        <v>89</v>
+      </c>
+      <c r="D45" s="1">
+        <v>75</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>90</v>
+      </c>
+      <c r="C46" t="s">
+        <v>91</v>
+      </c>
+      <c r="D46" s="1">
+        <v>45</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>92</v>
+      </c>
+      <c r="C47" t="s">
+        <v>93</v>
+      </c>
+      <c r="D47" s="1">
+        <v>35</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" t="s">
+        <v>95</v>
+      </c>
+      <c r="D48" s="1">
+        <v>85</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>86</v>
+      </c>
+      <c r="C49" t="s">
+        <v>87</v>
+      </c>
+      <c r="D49" s="1">
+        <v>70</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>96</v>
+      </c>
+      <c r="C50" t="s">
+        <v>97</v>
+      </c>
+      <c r="D50" s="1">
+        <v>55</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>98</v>
+      </c>
+      <c r="C51" t="s">
+        <v>99</v>
+      </c>
+      <c r="D51" s="1">
+        <v>45</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>100</v>
+      </c>
+      <c r="C52" t="s">
+        <v>101</v>
+      </c>
+      <c r="D52" s="1">
+        <v>40</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>102</v>
+      </c>
+      <c r="C53" t="s">
+        <v>103</v>
+      </c>
+      <c r="D53" s="1">
+        <v>75</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>104</v>
+      </c>
+      <c r="C54" t="s">
+        <v>105</v>
+      </c>
+      <c r="D54" s="1">
+        <v>60</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>106</v>
+      </c>
+      <c r="C55" t="s">
+        <v>107</v>
+      </c>
+      <c r="D55" s="1">
+        <v>75</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
+        <v>108</v>
+      </c>
+      <c r="C56" t="s">
+        <v>109</v>
+      </c>
+      <c r="D56" s="1">
+        <v>95</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>112</v>
+      </c>
+      <c r="C57" t="s">
+        <v>113</v>
+      </c>
+      <c r="D57" s="1">
+        <v>85</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
+        <v>110</v>
+      </c>
+      <c r="C58" t="s">
+        <v>111</v>
+      </c>
+      <c r="D58" s="1">
+        <v>50</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
+        <v>114</v>
+      </c>
+      <c r="C59" t="s">
+        <v>115</v>
+      </c>
+      <c r="D59" s="1">
+        <v>70</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
+        <v>116</v>
+      </c>
+      <c r="C60" t="s">
+        <v>117</v>
+      </c>
+      <c r="D60" s="1">
+        <v>55</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
+        <v>118</v>
+      </c>
+      <c r="C61" t="s">
+        <v>119</v>
+      </c>
+      <c r="D61" s="1">
+        <v>55</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
+        <v>120</v>
+      </c>
+      <c r="C62" t="s">
+        <v>121</v>
+      </c>
+      <c r="D62" s="1">
+        <v>70</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
+        <v>122</v>
+      </c>
+      <c r="C63" t="s">
+        <v>123</v>
+      </c>
+      <c r="D63" s="1">
+        <v>50</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B64" t="s">
+        <v>124</v>
+      </c>
+      <c r="C64" t="s">
+        <v>125</v>
+      </c>
+      <c r="D64" s="1">
+        <v>40</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
+        <v>126</v>
+      </c>
+      <c r="C65" t="s">
+        <v>127</v>
+      </c>
+      <c r="D65" s="1">
+        <v>55</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
+        <v>130</v>
+      </c>
+      <c r="C66" t="s">
+        <v>131</v>
+      </c>
+      <c r="D66" s="1">
+        <v>50</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B67" t="s">
+        <v>132</v>
+      </c>
+      <c r="C67" t="s">
+        <v>133</v>
+      </c>
+      <c r="D67" s="1">
+        <v>70</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B68" t="s">
+        <v>134</v>
+      </c>
+      <c r="C68" t="s">
+        <v>135</v>
+      </c>
+      <c r="D68" s="1">
+        <v>70</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B69" t="s">
+        <v>128</v>
+      </c>
+      <c r="C69" t="s">
+        <v>129</v>
+      </c>
+      <c r="D69" s="1">
+        <v>75</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
+        <v>136</v>
+      </c>
+      <c r="C70" t="s">
+        <v>137</v>
+      </c>
+      <c r="D70" s="1">
+        <v>78</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B71" t="s">
+        <v>138</v>
+      </c>
+      <c r="C71" t="s">
+        <v>139</v>
+      </c>
+      <c r="D71" s="1">
+        <v>75</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B72" t="s">
+        <v>140</v>
+      </c>
+      <c r="C72" t="s">
+        <v>141</v>
+      </c>
+      <c r="D72" s="1">
+        <v>80</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="B2:E72">
+    <sortCondition ref="C2:C72"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>